<commit_message>
update for March changing subscriptions:
</commit_message>
<xml_diff>
--- a/update_products.xlsx
+++ b/update_products.xlsx
@@ -33,13 +33,13 @@
     <t>shopify_variant_id</t>
   </si>
   <si>
-    <t>La Vie En Rose - 3 Item</t>
-  </si>
-  <si>
-    <t>La Vie En Rose - 5 Item</t>
-  </si>
-  <si>
     <t>product_collection</t>
+  </si>
+  <si>
+    <t>In The Zone - 3 Items</t>
+  </si>
+  <si>
+    <t>In The Zone - 5 Items</t>
   </si>
 </sst>
 </file>
@@ -50,13 +50,28 @@
     <numFmt numFmtId="164" formatCode="#######################00000"/>
     <numFmt numFmtId="165" formatCode="#######00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -77,15 +92,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,7 +437,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -443,45 +462,46 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>722457911059</v>
+        <v>764204132003</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>138427301906</v>
+        <v>175540207634</v>
       </c>
       <c r="D2" s="2">
-        <v>1340705931282</v>
+        <v>1599416074258</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>722457572946</v>
+        <v>764204132010</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>138427203602</v>
+        <v>175535685650</v>
       </c>
       <c r="D3" s="2">
-        <v>1340704751634</v>
+        <v>1599409848338</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updates for June 2018
</commit_message>
<xml_diff>
--- a/update_products.xlsx
+++ b/update_products.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FWallace/Shopify/update_subs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7703FD24-BA70-3744-B336-A61DCAFFC217}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="460" windowWidth="25360" windowHeight="18780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4460" yWindow="460" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>sku</t>
   </si>
@@ -42,16 +36,22 @@
     <t>product_collection</t>
   </si>
   <si>
-    <t>May Flowers - 5 Items</t>
-  </si>
-  <si>
-    <t>May Flowers - 3 Items</t>
+    <t>Rosé All Day - 3 Items</t>
+  </si>
+  <si>
+    <t>Rosé All Day - 5 Items</t>
+  </si>
+  <si>
+    <t>Rose All Day - 5 Items</t>
+  </si>
+  <si>
+    <t>Rose All Day - 3 Items</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#######################00000"/>
     <numFmt numFmtId="165" formatCode="#######00000"/>
@@ -447,14 +447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
@@ -462,7 +462,7 @@
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,38 +479,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>764204150236</v>
+        <v>764204172474</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>207131279378</v>
+        <v>224674119698</v>
       </c>
       <c r="D2" s="2">
-        <v>1819796963346</v>
+        <v>2008926027794</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>764204150243</v>
+        <v>764204172467</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>207131443218</v>
+        <v>224674086930</v>
       </c>
       <c r="D3" s="2">
-        <v>1819797192722</v>
+        <v>2008925995026</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>